<commit_message>
Creeated two code test cases for CAM-734 under story AIP-491
</commit_message>
<xml_diff>
--- a/Carrick_AutomatedTest/Carrick_Automation/TestData/CAM_729_730_731_733.xlsx
+++ b/Carrick_AutomatedTest/Carrick_Automation/TestData/CAM_729_730_731_733.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B65D79C-1E8B-42AF-8AFC-A38F3372086F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFE16805-B65F-4442-ADF1-5AF1DD724516}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20616" yWindow="-120" windowWidth="20736" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -439,28 +439,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="13.85546875" customWidth="1"/>
-    <col min="11" max="11" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="13.88671875" customWidth="1"/>
+    <col min="11" max="11" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -510,7 +510,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -560,7 +560,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -610,7 +610,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -660,7 +660,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
AIP-491 AIP-997 Undo changes(if any) to Carrick_AutomatedTest/Carrick_Automation/TestData/CAM_729_730_731_733.xlsx
</commit_message>
<xml_diff>
--- a/Carrick_AutomatedTest/Carrick_Automation/TestData/CAM_729_730_731_733.xlsx
+++ b/Carrick_AutomatedTest/Carrick_Automation/TestData/CAM_729_730_731_733.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFE16805-B65F-4442-ADF1-5AF1DD724516}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B65D79C-1E8B-42AF-8AFC-A38F3372086F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20616" yWindow="-120" windowWidth="20736" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -439,28 +439,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="13.88671875" customWidth="1"/>
-    <col min="11" max="11" width="23.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="13.85546875" customWidth="1"/>
+    <col min="11" max="11" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -510,7 +510,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -560,7 +560,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -610,7 +610,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -660,7 +660,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>

</xml_diff>